<commit_message>
chore: Add .gitignore and requirements.txt files
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandrovelazco/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandrovelazco/work/experimental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B997EF7-4D80-9845-92EA-8E08518F4C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70F109C-B55D-804D-843F-B04AAD6D9C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{C2427356-61DA-6A44-B1AE-9481182B87D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{C2427356-61DA-6A44-B1AE-9481182B87D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="226">
   <si>
     <t>token</t>
   </si>
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1768,11 +1768,21 @@
       <c r="B29" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">

</xml_diff>